<commit_message>
Updating to make ELO lowercase
</commit_message>
<xml_diff>
--- a/Rankings_Table.xlsx
+++ b/Rankings_Table.xlsx
@@ -446,7 +446,7 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>ELO</t>
+          <t>Elo</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
@@ -475,7 +475,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>1681</v>
+        <v>1684</v>
       </c>
       <c r="D2" t="n">
         <v>7</v>
@@ -497,7 +497,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>1676</v>
+        <v>1678</v>
       </c>
       <c r="D3" t="n">
         <v>5</v>
@@ -519,7 +519,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1676</v>
+        <v>1670</v>
       </c>
       <c r="D4" t="n">
         <v>6</v>
@@ -537,20 +537,20 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Eric Papa</t>
+          <t>Nelson Bakerman</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>1632</v>
+        <v>1640</v>
       </c>
       <c r="D5" t="n">
         <v>4</v>
       </c>
       <c r="E5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F5" t="n">
-        <v>0.667</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="6">
@@ -559,20 +559,20 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Nelson Bakerman</t>
+          <t>Chris Widgren</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>1629</v>
+        <v>1632</v>
       </c>
       <c r="D6" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>0.75</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
@@ -581,11 +581,11 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Jeff Ziev</t>
+          <t>Eric Papa</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>1629</v>
+        <v>1631</v>
       </c>
       <c r="D7" t="n">
         <v>4</v>
@@ -603,20 +603,20 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Ryan Leggette</t>
+          <t>Jeff Ziev</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>1626</v>
+        <v>1630</v>
       </c>
       <c r="D8" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E8" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F8" t="n">
-        <v>0.75</v>
+        <v>0.667</v>
       </c>
     </row>
     <row r="9">
@@ -625,20 +625,20 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Jeff Weber</t>
+          <t>Ryan Leggette</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>1618</v>
+        <v>1627</v>
       </c>
       <c r="D9" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E9" t="n">
         <v>1</v>
       </c>
       <c r="F9" t="n">
-        <v>0.667</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="10">
@@ -647,7 +647,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Justin Goodfellow</t>
+          <t>Bob Sauchelli</t>
         </is>
       </c>
       <c r="C10" t="n">
@@ -665,33 +665,33 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>David Chester</t>
+          <t>Paul Assad</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>1616</v>
+        <v>1617</v>
       </c>
       <c r="D11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11" t="n">
-        <v>1</v>
+        <v>0.667</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Chris Widgren</t>
+          <t>David Chester</t>
         </is>
       </c>
       <c r="C12" t="n">
@@ -709,7 +709,7 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -735,7 +735,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Paul Assad</t>
+          <t>Justin Goodfellow</t>
         </is>
       </c>
       <c r="C14" t="n">
@@ -757,33 +757,33 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Tom Witteman</t>
+          <t>Anthony Buccellato</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>1601</v>
+        <v>1613</v>
       </c>
       <c r="D15" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E15" t="n">
         <v>1</v>
       </c>
       <c r="F15" t="n">
-        <v>0.5</v>
+        <v>0.667</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>George Brown</t>
+          <t>Damir Uzunic</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>1601</v>
+        <v>1602</v>
       </c>
       <c r="D16" t="n">
         <v>1</v>
@@ -797,11 +797,11 @@
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Paul Jones</t>
+          <t>Isaac Dunn</t>
         </is>
       </c>
       <c r="C17" t="n">
@@ -819,21 +819,21 @@
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Adam Fratino</t>
+          <t>Paul Jones</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>1600</v>
+        <v>1601</v>
       </c>
       <c r="D18" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E18" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F18" t="n">
         <v>0.5</v>
@@ -841,11 +841,11 @@
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Bob Sauchelli</t>
+          <t>Kurowska</t>
         </is>
       </c>
       <c r="C19" t="n">
@@ -863,11 +863,11 @@
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Isaac Dunn</t>
+          <t>Tom Witteman</t>
         </is>
       </c>
       <c r="C20" t="n">
@@ -885,11 +885,11 @@
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Kurowska</t>
+          <t>Mike Brady</t>
         </is>
       </c>
       <c r="C21" t="n">
@@ -911,17 +911,17 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Colin Kelly</t>
+          <t>Ian Ainley</t>
         </is>
       </c>
       <c r="C22" t="n">
         <v>1599</v>
       </c>
       <c r="D22" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E22" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F22" t="n">
         <v>0.5</v>
@@ -933,7 +933,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Judy O'Brien</t>
+          <t>Colin Kelly</t>
         </is>
       </c>
       <c r="C23" t="n">
@@ -951,21 +951,21 @@
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Mike Brady</t>
+          <t>Adam Fratino</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>1599</v>
+        <v>1598</v>
       </c>
       <c r="D24" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E24" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F24" t="n">
         <v>0.5</v>
@@ -977,17 +977,17 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Ian Ainley</t>
+          <t>Judy O'Brien</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>1598</v>
+        <v>1597</v>
       </c>
       <c r="D25" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E25" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F25" t="n">
         <v>0.5</v>
@@ -995,68 +995,68 @@
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Ben Cole</t>
+          <t>Jeff Weber</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>1598</v>
+        <v>1588</v>
       </c>
       <c r="D26" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E26" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F26" t="n">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Matt Bird</t>
+          <t>George Brown</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>1598</v>
+        <v>1585</v>
       </c>
       <c r="D27" t="n">
         <v>1</v>
       </c>
       <c r="E27" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F27" t="n">
-        <v>0.5</v>
+        <v>0.333</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Damir Uzunic</t>
+          <t>Steve Olsen</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>1587</v>
+        <v>1585</v>
       </c>
       <c r="D28" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E28" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F28" t="n">
-        <v>0</v>
+        <v>0.333</v>
       </c>
     </row>
     <row r="29">
@@ -1065,25 +1065,25 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Steve Olsen</t>
+          <t>Dave Hitchings</t>
         </is>
       </c>
       <c r="C29" t="n">
         <v>1585</v>
       </c>
       <c r="D29" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E29" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F29" t="n">
-        <v>0.333</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
@@ -1105,11 +1105,11 @@
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Colin Hanson</t>
+          <t>Chris Greene</t>
         </is>
       </c>
       <c r="C31" t="n">
@@ -1153,7 +1153,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Kofi Wilson</t>
+          <t>Colin Hanson</t>
         </is>
       </c>
       <c r="C33" t="n">
@@ -1175,7 +1175,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Demelo</t>
+          <t>Kofi Wilson</t>
         </is>
       </c>
       <c r="C34" t="n">
@@ -1219,7 +1219,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Jeff Behrens</t>
+          <t>Demelo</t>
         </is>
       </c>
       <c r="C36" t="n">
@@ -1241,7 +1241,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Chris Greene</t>
+          <t>Phil O'Brien</t>
         </is>
       </c>
       <c r="C37" t="n">
@@ -1263,7 +1263,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Phil O'Brien</t>
+          <t>Jeff Behrens</t>
         </is>
       </c>
       <c r="C38" t="n">
@@ -1281,51 +1281,51 @@
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Alyssa Bird</t>
+          <t>Ben Cole</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>1584</v>
+        <v>1583</v>
       </c>
       <c r="D39" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E39" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F39" t="n">
-        <v>0</v>
+        <v>0.333</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Deb Czeresko</t>
+          <t>Roger Gibian</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>1584</v>
+        <v>1583</v>
       </c>
       <c r="D40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E40" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F40" t="n">
-        <v>0</v>
+        <v>0.333</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
@@ -1333,7 +1333,7 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>1584</v>
+        <v>1583</v>
       </c>
       <c r="D41" t="n">
         <v>0</v>
@@ -1347,15 +1347,15 @@
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Anthony Buccellato</t>
+          <t>Deb Czeresko</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>1584</v>
+        <v>1583</v>
       </c>
       <c r="D42" t="n">
         <v>0</v>
@@ -1369,15 +1369,15 @@
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Dave Hitchings</t>
+          <t>Amelia Burger</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>1584</v>
+        <v>1583</v>
       </c>
       <c r="D43" t="n">
         <v>0</v>
@@ -1395,20 +1395,20 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Amelia Burger</t>
+          <t>Matt Bird</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>1583</v>
+        <v>1582</v>
       </c>
       <c r="D44" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E44" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F44" t="n">
-        <v>0</v>
+        <v>0.333</v>
       </c>
     </row>
     <row r="45">
@@ -1421,7 +1421,7 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>1582</v>
+        <v>1581</v>
       </c>
       <c r="D45" t="n">
         <v>1</v>
@@ -1435,33 +1435,33 @@
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Roger Gibian</t>
+          <t>Pat Murphy</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>1582</v>
+        <v>1568</v>
       </c>
       <c r="D46" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E46" t="n">
         <v>2</v>
       </c>
       <c r="F46" t="n">
-        <v>0.333</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Dana Vandagriff</t>
+          <t>Alyssa Bird</t>
         </is>
       </c>
       <c r="C47" t="n">
@@ -1479,15 +1479,15 @@
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Pat Murphy</t>
+          <t>Dana Vandagriff</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>1568</v>
+        <v>1567</v>
       </c>
       <c r="D48" t="n">
         <v>0</v>
@@ -1501,7 +1501,7 @@
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
@@ -1553,7 +1553,7 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>1552</v>
+        <v>1553</v>
       </c>
       <c r="D51" t="n">
         <v>0</v>

</xml_diff>